<commit_message>
june + st98 graph
</commit_message>
<xml_diff>
--- a/Oil_current.xlsx
+++ b/Oil_current.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Information Management\Info Sharing and Tracking\Product Services\Operations\Product Creation\ST3\ST3s_Report_Prep\All_Pages_Content_Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eub.gov.ab.ca\CalFsrv\share0\Information Management\Info Sharing and Tracking\Product Services\Operations\Product Creation\ST3\ST3s_Report_Prep\All_Pages_Content_Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A49D5B-C35E-4EF0-A567-2E071D44B502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2856CE12-27A1-44B6-A56D-C40BE190D225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3615" yWindow="2940" windowWidth="21600" windowHeight="10650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="21" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="130">
   <si>
     <t>Reporting Adjustment</t>
   </si>
@@ -479,7 +479,7 @@
     <t/>
   </si>
   <si>
-    <t xml:space="preserve"> Run Date:  28 April 2025</t>
+    <t xml:space="preserve"> Run Date:  29 July 2025</t>
   </si>
 </sst>
 </file>
@@ -487,12 +487,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.00_)"/>
-    <numFmt numFmtId="167" formatCode="0____"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="0.00_)"/>
+    <numFmt numFmtId="168" formatCode="0____"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -805,14 +805,14 @@
   </borders>
   <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="4" fontId="11" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0">
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="40" fontId="13" fillId="0" borderId="0">
@@ -823,7 +823,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="168" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="39" fontId="17" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
@@ -848,23 +848,23 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -876,13 +876,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="6"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -892,7 +892,7 @@
       <alignment horizontal="left" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -912,15 +912,15 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -929,13 +929,13 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="27" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -966,13 +966,13 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="6"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -981,8 +981,8 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -995,63 +995,67 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="6"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="29" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="29" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1060,10 +1064,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -1626,11 +1626,11 @@
     </row>
     <row r="3" spans="1:63" s="2" customFormat="1" ht="19.5" customHeight="1">
       <c r="G3" s="33"/>
-      <c r="H3" s="104" t="s">
+      <c r="H3" s="106" t="s">
         <v>120</v>
       </c>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
+      <c r="I3" s="106"/>
+      <c r="J3" s="106"/>
       <c r="K3" s="34"/>
       <c r="M3" s="2" t="s">
         <v>38</v>
@@ -2800,8 +2800,8 @@
   </sheetPr>
   <dimension ref="B1:V89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75:Q78"/>
+    <sheetView tabSelected="1" topLeftCell="B23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O73" sqref="O73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2831,11 +2831,11 @@
     </row>
     <row r="3" spans="2:22" s="2" customFormat="1" ht="19.5" customHeight="1">
       <c r="G3" s="33"/>
-      <c r="H3" s="104" t="s">
+      <c r="H3" s="106" t="s">
         <v>120</v>
       </c>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
+      <c r="I3" s="106"/>
+      <c r="J3" s="106"/>
       <c r="K3" s="34"/>
       <c r="Q3"/>
     </row>
@@ -2917,22 +2917,22 @@
       </c>
       <c r="C7"/>
       <c r="D7" s="90">
-        <v>9506655</v>
+        <v>9506598</v>
       </c>
       <c r="E7" s="16">
-        <v>9473819.8000000007</v>
+        <v>9473799.9000000004</v>
       </c>
       <c r="F7" s="16">
-        <v>8542752.5999999996</v>
+        <v>8863606.3000000007</v>
       </c>
       <c r="G7" s="16">
-        <v>0</v>
+        <v>9166837.3000000007</v>
       </c>
       <c r="H7" s="16">
-        <v>0</v>
+        <v>10019694.4</v>
       </c>
       <c r="I7" s="16">
-        <v>0</v>
+        <v>9437852.5999999996</v>
       </c>
       <c r="J7" s="16">
         <v>0</v>
@@ -2954,7 +2954,7 @@
       </c>
       <c r="P7" s="8"/>
       <c r="Q7" s="91">
-        <v>9506655</v>
+        <v>9506598</v>
       </c>
       <c r="V7" s="16"/>
     </row>
@@ -3018,22 +3018,22 @@
         <v>25</v>
       </c>
       <c r="D11" s="90">
-        <v>1582847.5</v>
+        <v>1524538.4</v>
       </c>
       <c r="E11" s="16">
-        <v>1448289.5</v>
+        <v>1394865.1</v>
       </c>
       <c r="F11" s="16">
-        <v>1694687.9</v>
+        <v>1627739.4</v>
       </c>
       <c r="G11" s="16">
-        <v>0</v>
+        <v>1596329.4</v>
       </c>
       <c r="H11" s="16">
-        <v>0</v>
+        <v>1608253.5</v>
       </c>
       <c r="I11" s="16">
-        <v>0</v>
+        <v>1545285.8</v>
       </c>
       <c r="J11" s="16">
         <v>0</v>
@@ -3055,7 +3055,7 @@
       </c>
       <c r="P11" s="8"/>
       <c r="Q11" s="91">
-        <v>4725824.9000000004</v>
+        <v>9297011.6000000015</v>
       </c>
     </row>
     <row r="12" spans="2:22" s="1" customFormat="1">
@@ -3064,22 +3064,22 @@
       </c>
       <c r="C12"/>
       <c r="D12" s="90">
-        <v>347900.5</v>
+        <v>370010</v>
       </c>
       <c r="E12" s="16">
-        <v>307732.8</v>
+        <v>324940.79999999999</v>
       </c>
       <c r="F12" s="16">
-        <v>347514.2</v>
+        <v>370805.3</v>
       </c>
       <c r="G12" s="16">
-        <v>0</v>
+        <v>363028.3</v>
       </c>
       <c r="H12" s="16">
-        <v>0</v>
+        <v>363259.9</v>
       </c>
       <c r="I12" s="16">
-        <v>0</v>
+        <v>333382.40000000002</v>
       </c>
       <c r="J12" s="16">
         <v>0</v>
@@ -3101,7 +3101,7 @@
       </c>
       <c r="P12" s="8"/>
       <c r="Q12" s="91">
-        <v>1003147.5</v>
+        <v>2125426.7000000002</v>
       </c>
     </row>
     <row r="13" spans="2:22">
@@ -3109,22 +3109,22 @@
         <v>27</v>
       </c>
       <c r="D13" s="90">
-        <v>165494.9</v>
+        <v>169594.5</v>
       </c>
       <c r="E13" s="16">
-        <v>148119.29999999999</v>
+        <v>151254.29999999999</v>
       </c>
       <c r="F13" s="16">
-        <v>168204.7</v>
+        <v>171935.5</v>
       </c>
       <c r="G13" s="16">
-        <v>0</v>
+        <v>161818.29999999999</v>
       </c>
       <c r="H13" s="16">
-        <v>0</v>
+        <v>165151.70000000001</v>
       </c>
       <c r="I13" s="16">
-        <v>0</v>
+        <v>157909.79999999999</v>
       </c>
       <c r="J13" s="16">
         <v>0</v>
@@ -3146,7 +3146,7 @@
       </c>
       <c r="P13" s="8"/>
       <c r="Q13" s="91">
-        <v>481818.89999999997</v>
+        <v>977664.10000000009</v>
       </c>
     </row>
     <row r="14" spans="2:22">
@@ -3154,22 +3154,22 @@
         <v>122</v>
       </c>
       <c r="D14" s="97">
-        <v>613885.6</v>
+        <v>645954.5</v>
       </c>
       <c r="E14" s="76">
-        <v>545817</v>
+        <v>578615</v>
       </c>
       <c r="F14" s="76">
-        <v>598747.30000000005</v>
+        <v>638467.1</v>
       </c>
       <c r="G14" s="75">
-        <v>0</v>
+        <v>612962.30000000005</v>
       </c>
       <c r="H14" s="75">
-        <v>0</v>
+        <v>620296.69999999995</v>
       </c>
       <c r="I14" s="75">
-        <v>0</v>
+        <v>606565.80000000005</v>
       </c>
       <c r="J14" s="75">
         <v>0</v>
@@ -3191,7 +3191,7 @@
       </c>
       <c r="P14" s="76"/>
       <c r="Q14" s="97">
-        <v>1758449.9000000001</v>
+        <v>3702861.4000000004</v>
       </c>
     </row>
     <row r="15" spans="2:22" s="1" customFormat="1">
@@ -3199,22 +3199,22 @@
         <v>114</v>
       </c>
       <c r="D15" s="90">
-        <v>2710128.5</v>
+        <v>2710097.4</v>
       </c>
       <c r="E15" s="16">
-        <v>2449958.6</v>
+        <v>2449675.2000000002</v>
       </c>
       <c r="F15" s="16">
-        <v>2809154.0999999996</v>
+        <v>2808947.3000000003</v>
       </c>
       <c r="G15" s="16">
-        <v>0</v>
+        <v>2734138.3</v>
       </c>
       <c r="H15" s="16">
-        <v>0</v>
+        <v>2756961.8</v>
       </c>
       <c r="I15" s="16">
-        <v>0</v>
+        <v>2643143.8000000003</v>
       </c>
       <c r="J15" s="16">
         <v>0</v>
@@ -3236,7 +3236,7 @@
       </c>
       <c r="P15" s="8"/>
       <c r="Q15" s="91">
-        <v>7969241.2000000011</v>
+        <v>16102963.800000001</v>
       </c>
     </row>
     <row r="16" spans="2:22" s="1" customFormat="1">
@@ -3261,22 +3261,22 @@
         <v>30</v>
       </c>
       <c r="D17" s="90">
-        <v>413914.5</v>
+        <v>413767.6</v>
       </c>
       <c r="E17" s="16">
-        <v>357432.9</v>
+        <v>357469.6</v>
       </c>
       <c r="F17" s="16">
-        <v>392124.4</v>
+        <v>392222.9</v>
       </c>
       <c r="G17" s="16">
-        <v>0</v>
+        <v>420454.7</v>
       </c>
       <c r="H17" s="16">
-        <v>0</v>
+        <v>441560.6</v>
       </c>
       <c r="I17" s="16">
-        <v>0</v>
+        <v>386046.8</v>
       </c>
       <c r="J17" s="16">
         <v>0</v>
@@ -3298,7 +3298,7 @@
       </c>
       <c r="P17" s="8"/>
       <c r="Q17" s="91">
-        <v>1163471.8</v>
+        <v>2411522.1999999997</v>
       </c>
     </row>
     <row r="18" spans="2:17">
@@ -3368,16 +3368,16 @@
         <v>8586573.8000000007</v>
       </c>
       <c r="F21" s="16">
-        <v>9674889.3000000007</v>
+        <v>9674675.1999999993</v>
       </c>
       <c r="G21" s="16">
-        <v>0</v>
+        <v>9111057.1999999993</v>
       </c>
       <c r="H21" s="16">
-        <v>0</v>
+        <v>8860121.3000000007</v>
       </c>
       <c r="I21" s="16">
-        <v>0</v>
+        <v>8770133.1999999993</v>
       </c>
       <c r="J21" s="16">
         <v>0</v>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="P21" s="8"/>
       <c r="Q21" s="91">
-        <v>27894367.699999999</v>
+        <v>54635465.299999997</v>
       </c>
     </row>
     <row r="22" spans="2:17">
@@ -3417,13 +3417,13 @@
         <v>8814790.6999999993</v>
       </c>
       <c r="G22" s="16">
-        <v>0</v>
+        <v>7802331.9000000004</v>
       </c>
       <c r="H22" s="16">
-        <v>0</v>
+        <v>6619318</v>
       </c>
       <c r="I22" s="16">
-        <v>0</v>
+        <v>8448607.8000000007</v>
       </c>
       <c r="J22" s="16">
         <v>0</v>
@@ -3445,7 +3445,7 @@
       </c>
       <c r="P22" s="8"/>
       <c r="Q22" s="91">
-        <v>25132409.399999999</v>
+        <v>48002667.099999994</v>
       </c>
     </row>
     <row r="23" spans="2:17">
@@ -3460,16 +3460,16 @@
         <v>-6874941.5999999996</v>
       </c>
       <c r="F23" s="16">
-        <v>-6073582.4000000004</v>
+        <v>-7772361</v>
       </c>
       <c r="G23" s="16">
-        <v>0</v>
+        <v>-6629495.7999999998</v>
       </c>
       <c r="H23" s="16">
-        <v>0</v>
+        <v>-5503172.9000000004</v>
       </c>
       <c r="I23" s="16">
-        <v>0</v>
+        <v>-6572086.0999999996</v>
       </c>
       <c r="J23" s="16">
         <v>0</v>
@@ -3491,7 +3491,7 @@
       </c>
       <c r="P23" s="8"/>
       <c r="Q23" s="91">
-        <v>-21033552.299999997</v>
+        <v>-41437085.700000003</v>
       </c>
     </row>
     <row r="24" spans="2:17">
@@ -3506,16 +3506,16 @@
         <v>9086275.5000000019</v>
       </c>
       <c r="F24" s="16">
-        <v>12416097.6</v>
+        <v>10717104.899999999</v>
       </c>
       <c r="G24" s="16">
-        <v>0</v>
+        <v>10283893.300000001</v>
       </c>
       <c r="H24" s="16">
-        <v>0</v>
+        <v>9976266.4000000004</v>
       </c>
       <c r="I24" s="16">
-        <v>0</v>
+        <v>10646654.9</v>
       </c>
       <c r="J24" s="16">
         <v>0</v>
@@ -3537,7 +3537,7 @@
       </c>
       <c r="P24" s="8"/>
       <c r="Q24" s="91">
-        <v>31993224.799999997</v>
+        <v>61201046.699999988</v>
       </c>
     </row>
     <row r="25" spans="2:17">
@@ -3551,16 +3551,16 @@
         <v>5987292.2000000002</v>
       </c>
       <c r="F25" s="42">
-        <v>5013348.3</v>
+        <v>6742676.0999999996</v>
       </c>
       <c r="G25" s="42">
-        <v>0</v>
+        <v>5647824.0999999996</v>
       </c>
       <c r="H25" s="42">
-        <v>0</v>
+        <v>4600579.5999999996</v>
       </c>
       <c r="I25" s="42">
-        <v>0</v>
+        <v>5698414.5</v>
       </c>
       <c r="J25" s="42">
         <v>0</v>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="P25" s="8"/>
       <c r="Q25" s="99">
-        <v>18042207.699999999</v>
+        <v>35718353.700000003</v>
       </c>
     </row>
     <row r="26" spans="2:17">
@@ -3596,16 +3596,16 @@
         <v>15073567.700000003</v>
       </c>
       <c r="F26" s="16">
-        <v>17429445.899999999</v>
+        <v>17459781</v>
       </c>
       <c r="G26" s="16">
-        <v>0</v>
+        <v>15931717.4</v>
       </c>
       <c r="H26" s="16">
-        <v>0</v>
+        <v>14576846</v>
       </c>
       <c r="I26" s="16">
-        <v>0</v>
+        <v>16345069.4</v>
       </c>
       <c r="J26" s="16">
         <v>0</v>
@@ -3627,7 +3627,7 @@
       </c>
       <c r="P26" s="8"/>
       <c r="Q26" s="91">
-        <v>50035432.5</v>
+        <v>96919400.399999991</v>
       </c>
     </row>
     <row r="27" spans="2:17">
@@ -3653,22 +3653,22 @@
       </c>
       <c r="C28" s="17"/>
       <c r="D28" s="90">
-        <v>20656461.899999999</v>
+        <v>20656283.899999999</v>
       </c>
       <c r="E28" s="16">
-        <v>17880959.200000003</v>
+        <v>17880712.500000004</v>
       </c>
       <c r="F28" s="16">
-        <v>20630724.399999999</v>
+        <v>20660951.199999999</v>
       </c>
       <c r="G28" s="16">
-        <v>0</v>
+        <v>19086310.399999999</v>
       </c>
       <c r="H28" s="16">
-        <v>0</v>
+        <v>17775368.400000002</v>
       </c>
       <c r="I28" s="16">
-        <v>0</v>
+        <v>19374260</v>
       </c>
       <c r="J28" s="16">
         <v>0</v>
@@ -3690,7 +3690,7 @@
       </c>
       <c r="P28" s="8"/>
       <c r="Q28" s="90">
-        <v>59168145.5</v>
+        <v>115433886.39999999</v>
       </c>
     </row>
     <row r="29" spans="2:17">
@@ -3734,22 +3734,22 @@
         <v>49</v>
       </c>
       <c r="D31" s="90">
-        <v>1243092.6000000001</v>
+        <v>1243091</v>
       </c>
       <c r="E31" s="16">
-        <v>1071506.3999999999</v>
+        <v>1071466.1000000001</v>
       </c>
       <c r="F31" s="16">
-        <v>1276025.2</v>
+        <v>1274686.8999999999</v>
       </c>
       <c r="G31" s="16">
-        <v>0</v>
+        <v>1189741.8</v>
       </c>
       <c r="H31" s="16">
-        <v>0</v>
+        <v>1206795.8</v>
       </c>
       <c r="I31" s="16">
-        <v>0</v>
+        <v>1127360.8</v>
       </c>
       <c r="J31" s="16">
         <v>0</v>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="P31" s="8"/>
       <c r="Q31" s="91">
-        <v>3590624.2</v>
+        <v>7113142.3999999994</v>
       </c>
     </row>
     <row r="32" spans="2:17">
@@ -3788,13 +3788,13 @@
         <v>384891.6</v>
       </c>
       <c r="G32" s="16">
-        <v>0</v>
+        <v>373030.6</v>
       </c>
       <c r="H32" s="16">
-        <v>0</v>
+        <v>363016.5</v>
       </c>
       <c r="I32" s="16">
-        <v>0</v>
+        <v>325942.40000000002</v>
       </c>
       <c r="J32" s="16">
         <v>0</v>
@@ -3816,7 +3816,7 @@
       </c>
       <c r="P32" s="8"/>
       <c r="Q32" s="90">
-        <v>1118700</v>
+        <v>2180689.5</v>
       </c>
     </row>
     <row r="33" spans="2:17">
@@ -3848,16 +3848,16 @@
         <v>9839.6</v>
       </c>
       <c r="F34" s="16">
-        <v>11378.9</v>
+        <v>10997.5</v>
       </c>
       <c r="G34" s="16">
-        <v>0</v>
+        <v>11388.1</v>
       </c>
       <c r="H34" s="16">
-        <v>0</v>
+        <v>10958.3</v>
       </c>
       <c r="I34" s="16">
-        <v>0</v>
+        <v>9398.5</v>
       </c>
       <c r="J34" s="16">
         <v>0</v>
@@ -3879,7 +3879,7 @@
       </c>
       <c r="P34" s="8"/>
       <c r="Q34" s="91">
-        <v>32281.599999999999</v>
+        <v>63645.100000000006</v>
       </c>
     </row>
     <row r="35" spans="2:17">
@@ -3897,13 +3897,13 @@
         <v>11412.3</v>
       </c>
       <c r="G35" s="16">
-        <v>0</v>
+        <v>10763.4</v>
       </c>
       <c r="H35" s="16">
-        <v>0</v>
+        <v>7623.8</v>
       </c>
       <c r="I35" s="16">
-        <v>0</v>
+        <v>10365.799999999999</v>
       </c>
       <c r="J35" s="16">
         <v>0</v>
@@ -3925,7 +3925,7 @@
       </c>
       <c r="P35" s="8"/>
       <c r="Q35" s="91">
-        <v>25926.1</v>
+        <v>54679.100000000006</v>
       </c>
     </row>
     <row r="36" spans="2:17">
@@ -3934,22 +3934,22 @@
       </c>
       <c r="C36" s="17"/>
       <c r="D36" s="90">
-        <v>563893.19999999995</v>
+        <v>564149.80000000005</v>
       </c>
       <c r="E36" s="16">
-        <v>466223.5</v>
+        <v>466259.8</v>
       </c>
       <c r="F36" s="16">
-        <v>574558.4</v>
+        <v>574571.4</v>
       </c>
       <c r="G36" s="16">
-        <v>0</v>
+        <v>424637.2</v>
       </c>
       <c r="H36" s="16">
-        <v>0</v>
+        <v>298022.5</v>
       </c>
       <c r="I36" s="16">
-        <v>0</v>
+        <v>346930.1</v>
       </c>
       <c r="J36" s="16">
         <v>0</v>
@@ -3971,7 +3971,7 @@
       </c>
       <c r="P36" s="8"/>
       <c r="Q36" s="91">
-        <v>1604675.1</v>
+        <v>2674570.8000000003</v>
       </c>
     </row>
     <row r="37" spans="2:17">
@@ -4004,16 +4004,16 @@
         <v>244717.5</v>
       </c>
       <c r="F38" s="16">
-        <v>290996.2</v>
+        <v>291235.7</v>
       </c>
       <c r="G38" s="16">
-        <v>0</v>
+        <v>270068.3</v>
       </c>
       <c r="H38" s="16">
-        <v>0</v>
+        <v>214673.2</v>
       </c>
       <c r="I38" s="16">
-        <v>0</v>
+        <v>204350.4</v>
       </c>
       <c r="J38" s="16">
         <v>0</v>
@@ -4035,7 +4035,7 @@
       </c>
       <c r="P38" s="8"/>
       <c r="Q38" s="91">
-        <v>816282.5</v>
+        <v>1505613.9</v>
       </c>
     </row>
     <row r="39" spans="2:17">
@@ -4053,13 +4053,13 @@
         <v>51.9</v>
       </c>
       <c r="G39" s="16">
-        <v>0</v>
+        <v>107.5</v>
       </c>
       <c r="H39" s="16">
-        <v>0</v>
+        <v>82.2</v>
       </c>
       <c r="I39" s="16">
-        <v>0</v>
+        <v>26.5</v>
       </c>
       <c r="J39" s="16">
         <v>0</v>
@@ -4081,7 +4081,7 @@
       </c>
       <c r="P39" s="8"/>
       <c r="Q39" s="91">
-        <v>148.6</v>
+        <v>364.8</v>
       </c>
     </row>
     <row r="40" spans="2:17">
@@ -4137,13 +4137,13 @@
         <v>424953.5</v>
       </c>
       <c r="G42" s="78">
-        <v>0</v>
+        <v>486286.3</v>
       </c>
       <c r="H42" s="78">
-        <v>0</v>
+        <v>527931.4</v>
       </c>
       <c r="I42" s="78">
-        <v>0</v>
+        <v>459063.2</v>
       </c>
       <c r="J42" s="78">
         <v>0</v>
@@ -4165,8 +4165,7 @@
       </c>
       <c r="P42" s="79"/>
       <c r="Q42" s="79">
-        <f t="shared" ref="Q42:Q46" si="0">SUM(D42:O42)</f>
-        <v>1316134.7</v>
+        <v>2789415.6</v>
       </c>
     </row>
     <row r="43" spans="2:17">
@@ -4175,25 +4174,22 @@
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="78">
-        <f>545525.1+612469.9</f>
         <v>1157995</v>
       </c>
       <c r="E43" s="78">
-        <f>550137+548662.1</f>
         <v>1098799.1000000001</v>
       </c>
       <c r="F43" s="78">
-        <f>566495.6+582720</f>
         <v>1149215.6000000001</v>
       </c>
       <c r="G43" s="78">
-        <v>0</v>
+        <v>1176069</v>
       </c>
       <c r="H43" s="78">
-        <v>0</v>
+        <v>1260869.7</v>
       </c>
       <c r="I43" s="78">
-        <v>0</v>
+        <v>1109572.7</v>
       </c>
       <c r="J43" s="78">
         <v>0</v>
@@ -4215,8 +4211,7 @@
       </c>
       <c r="P43" s="79"/>
       <c r="Q43" s="79">
-        <f t="shared" si="0"/>
-        <v>3406009.7</v>
+        <v>6952521.0999999996</v>
       </c>
     </row>
     <row r="44" spans="2:17">
@@ -4225,22 +4220,22 @@
       </c>
       <c r="C44" s="18"/>
       <c r="D44" s="78">
-        <v>911490.1</v>
+        <v>911629.3</v>
       </c>
       <c r="E44" s="78">
-        <v>799614.7</v>
+        <v>799705.2</v>
       </c>
       <c r="F44" s="78">
-        <v>910303.4</v>
+        <v>910397.8</v>
       </c>
       <c r="G44" s="78">
-        <v>0</v>
+        <v>891385.3</v>
       </c>
       <c r="H44" s="78">
-        <v>0</v>
+        <v>769001</v>
       </c>
       <c r="I44" s="78">
-        <v>0</v>
+        <v>732303.1</v>
       </c>
       <c r="J44" s="78">
         <v>0</v>
@@ -4262,8 +4257,7 @@
       </c>
       <c r="P44" s="79"/>
       <c r="Q44" s="79">
-        <f t="shared" si="0"/>
-        <v>2621408.1999999997</v>
+        <v>5014421.6999999993</v>
       </c>
     </row>
     <row r="45" spans="2:17">
@@ -4281,13 +4275,13 @@
         <v>335457.90000000002</v>
       </c>
       <c r="G45" s="80">
-        <v>0</v>
+        <v>257566.2</v>
       </c>
       <c r="H45" s="80">
-        <v>0</v>
+        <v>320994.2</v>
       </c>
       <c r="I45" s="80">
-        <v>0</v>
+        <v>353975.6</v>
       </c>
       <c r="J45" s="80">
         <v>0</v>
@@ -4309,8 +4303,7 @@
       </c>
       <c r="P45" s="80"/>
       <c r="Q45" s="80">
-        <f t="shared" si="0"/>
-        <v>875222.3</v>
+        <v>1807758.2999999998</v>
       </c>
     </row>
     <row r="46" spans="2:17">
@@ -4319,25 +4312,22 @@
       </c>
       <c r="C46" s="17"/>
       <c r="D46" s="89">
-        <f t="shared" ref="D46:F46" si="1">SUM(D42:D45)</f>
-        <v>2851547.3</v>
+        <v>2851686.5</v>
       </c>
       <c r="E46" s="89">
-        <f t="shared" si="1"/>
-        <v>2547297.2000000002</v>
+        <v>2547387.7000000002</v>
       </c>
       <c r="F46" s="89">
-        <f t="shared" si="1"/>
-        <v>2819930.4</v>
+        <v>2820024.8</v>
       </c>
       <c r="G46" s="89">
-        <v>0</v>
+        <v>2811306.8</v>
       </c>
       <c r="H46" s="89">
-        <v>0</v>
+        <v>2878796.3</v>
       </c>
       <c r="I46" s="89">
-        <v>0</v>
+        <v>2654914.6</v>
       </c>
       <c r="J46" s="89">
         <v>0</v>
@@ -4359,8 +4349,7 @@
       </c>
       <c r="P46" s="79"/>
       <c r="Q46" s="79">
-        <f t="shared" si="0"/>
-        <v>8218774.9000000004</v>
+        <v>16564116.699999999</v>
       </c>
     </row>
     <row r="47" spans="2:17">
@@ -4386,25 +4375,22 @@
         <v>58</v>
       </c>
       <c r="D48" s="89">
-        <f t="shared" ref="D48:F48" si="2">D31+D32+D34+D35+D36+D38+D39+D46</f>
-        <v>5350514.5</v>
+        <v>5350908.7</v>
       </c>
       <c r="E48" s="89">
-        <f t="shared" si="2"/>
-        <v>4687653.5999999996</v>
+        <v>4687740.0999999996</v>
       </c>
       <c r="F48" s="89">
-        <f t="shared" si="2"/>
-        <v>5369244.9000000004</v>
+        <v>5367872.0999999996</v>
       </c>
       <c r="G48" s="89">
-        <v>0</v>
+        <v>5091043.7</v>
       </c>
       <c r="H48" s="89">
-        <v>0</v>
+        <v>4979968.5999999996</v>
       </c>
       <c r="I48" s="89">
-        <v>0</v>
+        <v>4679289.0999999996</v>
       </c>
       <c r="J48" s="89">
         <v>0</v>
@@ -4426,8 +4412,7 @@
       </c>
       <c r="P48" s="79"/>
       <c r="Q48" s="79">
-        <f>SUM(D48:O48)</f>
-        <v>15407413</v>
+        <v>30156822.300000001</v>
       </c>
     </row>
     <row r="49" spans="2:17">
@@ -4461,13 +4446,13 @@
         <v>215046.8</v>
       </c>
       <c r="G50" s="78">
-        <v>0</v>
+        <v>189681.1</v>
       </c>
       <c r="H50" s="78">
-        <v>0</v>
+        <v>172020.8</v>
       </c>
       <c r="I50" s="78">
-        <v>0</v>
+        <v>248140.7</v>
       </c>
       <c r="J50" s="78">
         <v>0</v>
@@ -4489,8 +4474,7 @@
       </c>
       <c r="P50" s="79"/>
       <c r="Q50" s="79">
-        <f t="shared" ref="Q50:Q52" si="3">SUM(D50:O50)</f>
-        <v>612639.60000000009</v>
+        <v>1222482.2</v>
       </c>
     </row>
     <row r="51" spans="2:17">
@@ -4501,19 +4485,19 @@
         <v>124236.8</v>
       </c>
       <c r="E51" s="78">
-        <v>115913.1</v>
+        <v>116058.3</v>
       </c>
       <c r="F51" s="78">
         <v>121794.8</v>
       </c>
       <c r="G51" s="78">
-        <v>0</v>
+        <v>106269.2</v>
       </c>
       <c r="H51" s="78">
-        <v>0</v>
+        <v>116208.9</v>
       </c>
       <c r="I51" s="78">
-        <v>0</v>
+        <v>110066.6</v>
       </c>
       <c r="J51" s="78">
         <v>0</v>
@@ -4535,8 +4519,7 @@
       </c>
       <c r="P51" s="79"/>
       <c r="Q51" s="79">
-        <f t="shared" si="3"/>
-        <v>361944.7</v>
+        <v>694634.6</v>
       </c>
     </row>
     <row r="52" spans="2:17">
@@ -4544,22 +4527,22 @@
         <v>17</v>
       </c>
       <c r="D52" s="78">
-        <v>356789.8</v>
+        <v>356815.3</v>
       </c>
       <c r="E52" s="78">
-        <v>315688.3</v>
+        <v>315710.5</v>
       </c>
       <c r="F52" s="78">
-        <v>370741.4</v>
+        <v>370577.6</v>
       </c>
       <c r="G52" s="78">
-        <v>0</v>
+        <v>346866.3</v>
       </c>
       <c r="H52" s="78">
-        <v>0</v>
+        <v>340015.4</v>
       </c>
       <c r="I52" s="78">
-        <v>0</v>
+        <v>333959.7</v>
       </c>
       <c r="J52" s="78">
         <v>0</v>
@@ -4581,27 +4564,26 @@
       </c>
       <c r="P52" s="78"/>
       <c r="Q52" s="78">
-        <f t="shared" si="3"/>
-        <v>1043219.5</v>
+        <v>2063944.8</v>
       </c>
     </row>
     <row r="53" spans="2:17" ht="14.25" customHeight="1">
       <c r="B53" s="50"/>
       <c r="C53" s="22"/>
-      <c r="D53" s="105"/>
-      <c r="E53" s="105"/>
-      <c r="F53" s="105"/>
-      <c r="G53" s="105"/>
-      <c r="H53" s="105"/>
-      <c r="I53" s="105"/>
-      <c r="J53" s="105"/>
-      <c r="K53" s="105"/>
-      <c r="L53" s="105"/>
-      <c r="M53" s="105"/>
-      <c r="N53" s="105"/>
-      <c r="O53" s="105"/>
-      <c r="P53" s="105"/>
-      <c r="Q53" s="106"/>
+      <c r="D53" s="102"/>
+      <c r="E53" s="102"/>
+      <c r="F53" s="102"/>
+      <c r="G53" s="102"/>
+      <c r="H53" s="102"/>
+      <c r="I53" s="102"/>
+      <c r="J53" s="102"/>
+      <c r="K53" s="102"/>
+      <c r="L53" s="102"/>
+      <c r="M53" s="102"/>
+      <c r="N53" s="102"/>
+      <c r="O53" s="102"/>
+      <c r="P53" s="102"/>
+      <c r="Q53" s="103"/>
     </row>
     <row r="54" spans="2:17" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="B54" s="50" t="s">
@@ -4609,22 +4591,22 @@
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="83">
-        <v>9473919.5</v>
+        <v>9473899.5999999996</v>
       </c>
       <c r="E54" s="83">
-        <v>8863692.4000000004</v>
+        <v>8863606.3000000007</v>
       </c>
       <c r="F54" s="83">
-        <v>8788273.5</v>
+        <v>9169358.4000000004</v>
       </c>
       <c r="G54" s="83">
-        <v>0</v>
+        <v>10019771.1</v>
       </c>
       <c r="H54" s="83">
-        <v>0</v>
+        <v>9476708.6999999993</v>
       </c>
       <c r="I54" s="83">
-        <v>0</v>
+        <v>9412626.1999999993</v>
       </c>
       <c r="J54" s="83">
         <v>0</v>
@@ -4646,7 +4628,7 @@
       </c>
       <c r="P54" s="83"/>
       <c r="Q54" s="84">
-        <v>8788273.5</v>
+        <v>9412626.1999999993</v>
       </c>
     </row>
     <row r="55" spans="2:17">
@@ -4654,22 +4636,22 @@
         <v>50</v>
       </c>
       <c r="D55" s="78">
-        <v>-242912.3</v>
+        <v>-243034.2</v>
       </c>
       <c r="E55" s="78">
-        <v>-139681.70000000001</v>
+        <v>-139906.9</v>
       </c>
       <c r="F55" s="78">
-        <v>403492.4</v>
+        <v>-142304</v>
       </c>
       <c r="G55" s="78">
-        <v>0</v>
+        <v>-87939.8</v>
       </c>
       <c r="H55" s="78">
-        <v>0</v>
+        <v>-338343.7</v>
       </c>
       <c r="I55" s="78">
-        <v>0</v>
+        <v>-318616.09999999998</v>
       </c>
       <c r="J55" s="78">
         <v>0</v>
@@ -4691,8 +4673,7 @@
       </c>
       <c r="P55" s="79"/>
       <c r="Q55" s="79">
-        <f>SUM(D55:O55)</f>
-        <v>20898.400000000023</v>
+        <v>-1270144.7000000002</v>
       </c>
     </row>
     <row r="56" spans="2:17" ht="15.75" thickBot="1">
@@ -4718,25 +4699,22 @@
         <v>31</v>
       </c>
       <c r="D57" s="89">
-        <f t="shared" ref="D57:F57" si="4">D7-D54+(D28+D48)-(D50+D51+D52)+D55</f>
-        <v>25092948.299999997</v>
+        <v>25092980</v>
       </c>
       <c r="E57" s="89">
-        <f t="shared" si="4"/>
-        <v>22432689.000000004</v>
+        <v>22432202.399999999</v>
       </c>
       <c r="F57" s="89">
-        <f t="shared" si="4"/>
-        <v>25450357.799999997</v>
+        <v>24873348</v>
       </c>
       <c r="G57" s="89">
-        <v>0</v>
+        <v>22593663.899999999</v>
       </c>
       <c r="H57" s="89">
-        <v>0</v>
+        <v>22331733.899999999</v>
       </c>
       <c r="I57" s="89">
-        <v>0</v>
+        <v>23067992.399999999</v>
       </c>
       <c r="J57" s="89">
         <v>0</v>
@@ -4758,8 +4736,7 @@
       </c>
       <c r="P57" s="79"/>
       <c r="Q57" s="79">
-        <f>SUM(D57:O57)</f>
-        <v>72975995.099999994</v>
+        <v>140391920.59999999</v>
       </c>
     </row>
     <row r="58" spans="2:17">
@@ -4784,20 +4761,20 @@
         <v>129</v>
       </c>
       <c r="C59" s="4"/>
-      <c r="D59" s="102"/>
-      <c r="E59" s="102"/>
-      <c r="F59" s="102"/>
-      <c r="G59" s="102"/>
-      <c r="H59" s="102"/>
-      <c r="I59" s="102"/>
-      <c r="J59" s="102"/>
-      <c r="K59" s="102"/>
-      <c r="L59" s="102"/>
-      <c r="M59" s="102"/>
-      <c r="N59" s="102"/>
-      <c r="O59" s="102"/>
-      <c r="P59" s="102"/>
-      <c r="Q59" s="103" t="s">
+      <c r="D59" s="104"/>
+      <c r="E59" s="104"/>
+      <c r="F59" s="104"/>
+      <c r="G59" s="104"/>
+      <c r="H59" s="104"/>
+      <c r="I59" s="104"/>
+      <c r="J59" s="104"/>
+      <c r="K59" s="104"/>
+      <c r="L59" s="104"/>
+      <c r="M59" s="104"/>
+      <c r="N59" s="104"/>
+      <c r="O59" s="104"/>
+      <c r="P59" s="104"/>
+      <c r="Q59" s="105" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4897,13 +4874,13 @@
         <v>69757.399999999994</v>
       </c>
       <c r="G63" s="90">
-        <v>0</v>
+        <v>38272</v>
       </c>
       <c r="H63" s="90">
-        <v>0</v>
+        <v>39155.9</v>
       </c>
       <c r="I63" s="90">
-        <v>0</v>
+        <v>60933.7</v>
       </c>
       <c r="J63" s="90">
         <v>0</v>
@@ -4925,7 +4902,7 @@
       </c>
       <c r="P63" s="91"/>
       <c r="Q63" s="91">
-        <v>169738</v>
+        <v>308099.59999999998</v>
       </c>
     </row>
     <row r="64" spans="2:17">
@@ -4942,13 +4919,13 @@
         <v>2517299.4</v>
       </c>
       <c r="G64" s="90">
-        <v>0</v>
+        <v>2118283.4</v>
       </c>
       <c r="H64" s="90">
-        <v>0</v>
+        <v>1988167.4</v>
       </c>
       <c r="I64" s="90">
-        <v>0</v>
+        <v>2219706</v>
       </c>
       <c r="J64" s="90">
         <v>0</v>
@@ -4970,7 +4947,7 @@
       </c>
       <c r="P64" s="91"/>
       <c r="Q64" s="91">
-        <v>7372289.0999999996</v>
+        <v>13698445.9</v>
       </c>
     </row>
     <row r="65" spans="2:17">
@@ -4978,22 +4955,22 @@
         <v>53</v>
       </c>
       <c r="D65" s="90">
-        <v>11271.4</v>
+        <v>11309</v>
       </c>
       <c r="E65" s="90">
-        <v>8492.6</v>
+        <v>8492.7000000000007</v>
       </c>
       <c r="F65" s="90">
-        <v>14430</v>
+        <v>14432.6</v>
       </c>
       <c r="G65" s="90">
-        <v>0</v>
+        <v>15261.8</v>
       </c>
       <c r="H65" s="90">
-        <v>0</v>
+        <v>11089.6</v>
       </c>
       <c r="I65" s="90">
-        <v>0</v>
+        <v>11993</v>
       </c>
       <c r="J65" s="90">
         <v>0</v>
@@ -5015,7 +4992,7 @@
       </c>
       <c r="P65" s="91"/>
       <c r="Q65" s="91">
-        <v>34194</v>
+        <v>72578.700000000012</v>
       </c>
     </row>
     <row r="66" spans="2:17">
@@ -5032,13 +5009,13 @@
         <v>15053.5</v>
       </c>
       <c r="G66" s="90">
-        <v>0</v>
+        <v>18091.8</v>
       </c>
       <c r="H66" s="90">
-        <v>0</v>
+        <v>19963.8</v>
       </c>
       <c r="I66" s="90">
-        <v>0</v>
+        <v>13665.6</v>
       </c>
       <c r="J66" s="90">
         <v>0</v>
@@ -5060,7 +5037,7 @@
       </c>
       <c r="P66" s="91"/>
       <c r="Q66" s="91">
-        <v>47547.8</v>
+        <v>99269.000000000015</v>
       </c>
     </row>
     <row r="67" spans="2:17" s="1" customFormat="1">
@@ -5078,13 +5055,13 @@
         <v>110.3</v>
       </c>
       <c r="G67" s="90">
-        <v>0</v>
+        <v>223</v>
       </c>
       <c r="H67" s="90">
         <v>0</v>
       </c>
       <c r="I67" s="90">
-        <v>0</v>
+        <v>338.9</v>
       </c>
       <c r="J67" s="90">
         <v>0</v>
@@ -5106,7 +5083,7 @@
       </c>
       <c r="P67" s="91"/>
       <c r="Q67" s="93">
-        <v>110.3</v>
+        <v>672.2</v>
       </c>
     </row>
     <row r="68" spans="2:17" s="1" customFormat="1">
@@ -5115,22 +5092,22 @@
       </c>
       <c r="C68" s="24"/>
       <c r="D68" s="90">
-        <v>-10575.2</v>
+        <v>-10715.4</v>
       </c>
       <c r="E68" s="90">
-        <v>20681.400000000001</v>
+        <v>20780.8</v>
       </c>
       <c r="F68" s="90">
-        <v>-1097.2</v>
+        <v>-1006.6</v>
       </c>
       <c r="G68" s="90">
-        <v>0</v>
+        <v>1167.5999999999999</v>
       </c>
       <c r="H68" s="90">
-        <v>0</v>
+        <v>11810.4</v>
       </c>
       <c r="I68" s="90">
-        <v>0</v>
+        <v>13105.2</v>
       </c>
       <c r="J68" s="90">
         <v>0</v>
@@ -5152,7 +5129,7 @@
       </c>
       <c r="P68" s="91"/>
       <c r="Q68" s="90">
-        <v>9009</v>
+        <v>35142</v>
       </c>
     </row>
     <row r="69" spans="2:17">
@@ -5167,16 +5144,16 @@
         <v>276205.40000000002</v>
       </c>
       <c r="F69" s="90">
-        <v>343276.4</v>
+        <v>341193.9</v>
       </c>
       <c r="G69" s="90">
-        <v>0</v>
+        <v>312016.59999999998</v>
       </c>
       <c r="H69" s="90">
-        <v>0</v>
+        <v>175192</v>
       </c>
       <c r="I69" s="90">
-        <v>0</v>
+        <v>206102.6</v>
       </c>
       <c r="J69" s="90">
         <v>0</v>
@@ -5198,7 +5175,7 @@
       </c>
       <c r="P69" s="91"/>
       <c r="Q69" s="91">
-        <v>966725.70000000007</v>
+        <v>1657954.4000000001</v>
       </c>
     </row>
     <row r="70" spans="2:17">
@@ -5207,22 +5184,22 @@
       </c>
       <c r="C70" s="19"/>
       <c r="D70" s="90">
-        <v>2951361.4</v>
+        <v>2951258.8000000003</v>
       </c>
       <c r="E70" s="90">
-        <v>2689422.7</v>
+        <v>2689522.2</v>
       </c>
       <c r="F70" s="90">
-        <v>2958829.7999999993</v>
+        <v>2956840.4999999995</v>
       </c>
       <c r="G70" s="90">
-        <v>0</v>
+        <v>2503316.1999999997</v>
       </c>
       <c r="H70" s="90">
-        <v>0</v>
+        <v>2245379.0999999996</v>
       </c>
       <c r="I70" s="90">
-        <v>0</v>
+        <v>2525845.0000000005</v>
       </c>
       <c r="J70" s="90">
         <v>0</v>
@@ -5244,7 +5221,7 @@
       </c>
       <c r="P70" s="91"/>
       <c r="Q70" s="91">
-        <v>8599613.8999999985</v>
+        <v>15872161.799999999</v>
       </c>
     </row>
     <row r="71" spans="2:17">
@@ -5280,13 +5257,13 @@
         <v>21577914.399999999</v>
       </c>
       <c r="G72" s="78">
-        <v>0</v>
+        <v>19669729.300000001</v>
       </c>
       <c r="H72" s="78">
-        <v>0</v>
+        <v>19906583.100000001</v>
       </c>
       <c r="I72" s="78">
-        <v>0</v>
+        <v>20283093.100000001</v>
       </c>
       <c r="J72" s="78">
         <v>0</v>
@@ -5308,7 +5285,7 @@
       </c>
       <c r="P72" s="79"/>
       <c r="Q72" s="79">
-        <v>62932581</v>
+        <v>122791986.5</v>
       </c>
     </row>
     <row r="73" spans="2:17">
@@ -5326,13 +5303,13 @@
         <v>696061.7548387096</v>
       </c>
       <c r="G73" s="78">
-        <v>0</v>
+        <v>655657.64333333331</v>
       </c>
       <c r="H73" s="78">
-        <v>0</v>
+        <v>642147.84193548397</v>
       </c>
       <c r="I73" s="78">
-        <v>0</v>
+        <v>676103.10333333339</v>
       </c>
       <c r="J73" s="78">
         <v>0</v>
@@ -5354,7 +5331,7 @@
       </c>
       <c r="P73" s="79"/>
       <c r="Q73" s="79">
-        <v>699264.77315668203</v>
+        <v>678617.15134536615</v>
       </c>
     </row>
     <row r="74" spans="2:17">
@@ -5381,25 +5358,22 @@
       </c>
       <c r="C75" s="17"/>
       <c r="D75" s="89">
-        <f t="shared" ref="D75:F75" si="5">D57-(D70+D72)</f>
-        <v>377987.39999999851</v>
+        <v>378121.7</v>
       </c>
       <c r="E75" s="89">
-        <f t="shared" si="5"/>
-        <v>152199.20000000298</v>
+        <v>151613.1</v>
       </c>
       <c r="F75" s="89">
-        <f t="shared" si="5"/>
-        <v>913613.59999999776</v>
+        <v>338593.1</v>
       </c>
       <c r="G75" s="89">
-        <v>0</v>
+        <v>420618.4</v>
       </c>
       <c r="H75" s="89">
-        <v>0</v>
+        <v>179771.7</v>
       </c>
       <c r="I75" s="89">
-        <v>0</v>
+        <v>259054.3</v>
       </c>
       <c r="J75" s="89">
         <v>0</v>
@@ -5421,8 +5395,7 @@
       </c>
       <c r="P75" s="79"/>
       <c r="Q75" s="79">
-        <f>SUM(D75:O75)</f>
-        <v>1443800.1999999993</v>
+        <v>1727772.3</v>
       </c>
     </row>
     <row r="76" spans="2:17">
@@ -5431,25 +5404,22 @@
       </c>
       <c r="C76" s="18"/>
       <c r="D76" s="94">
-        <f t="shared" ref="D76:F76" si="6">IF(D57&gt;0,D75/D57,"")</f>
-        <v>1.5063490964909793E-2</v>
+        <v>-5.664141253135831E-3</v>
       </c>
       <c r="E76" s="94">
-        <f t="shared" si="6"/>
-        <v>6.784706015404705E-3</v>
+        <v>-1.8147938447986213E-2</v>
       </c>
       <c r="F76" s="94">
-        <f t="shared" si="6"/>
-        <v>3.5897868594994678E-2</v>
-      </c>
-      <c r="G76" s="94" t="s">
-        <v>128</v>
-      </c>
-      <c r="H76" s="94" t="s">
-        <v>128</v>
-      </c>
-      <c r="I76" s="94" t="s">
-        <v>128</v>
+        <v>-1.0054176002127407E-2</v>
+      </c>
+      <c r="G76" s="94">
+        <v>-9.5774431002311582E-3</v>
+      </c>
+      <c r="H76" s="94">
+        <v>-2.3483407604001957E-2</v>
+      </c>
+      <c r="I76" s="94">
+        <v>-1.5572053579000338E-2</v>
       </c>
       <c r="J76" s="94" t="s">
         <v>128</v>
@@ -5471,8 +5441,7 @@
       </c>
       <c r="P76" s="94"/>
       <c r="Q76" s="95">
-        <f>AVERAGE(D76:O76)</f>
-        <v>1.9248688525103058E-2</v>
+        <v>-1.3513925313701844E-2</v>
       </c>
     </row>
     <row r="77" spans="2:17" ht="15.75" thickBot="1">
@@ -5498,25 +5467,22 @@
         <v>36</v>
       </c>
       <c r="D78" s="89">
-        <f t="shared" ref="D78:F78" si="7">(D70+D72)+D75</f>
-        <v>25092948.299999997</v>
+        <v>25092980</v>
       </c>
       <c r="E78" s="89">
-        <f t="shared" si="7"/>
-        <v>22432689.000000004</v>
+        <v>22432202.399999999</v>
       </c>
       <c r="F78" s="89">
-        <f t="shared" si="7"/>
-        <v>25450357.799999997</v>
+        <v>24873348</v>
       </c>
       <c r="G78" s="89">
-        <v>0</v>
+        <v>22593663.899999999</v>
       </c>
       <c r="H78" s="89">
-        <v>0</v>
+        <v>22331733.899999999</v>
       </c>
       <c r="I78" s="89">
-        <v>0</v>
+        <v>23067992.399999999</v>
       </c>
       <c r="J78" s="89">
         <v>0</v>
@@ -5538,8 +5504,7 @@
       </c>
       <c r="P78" s="79"/>
       <c r="Q78" s="79">
-        <f>SUM(D78:O78)</f>
-        <v>72975995.099999994</v>
+        <v>140391920.59999999</v>
       </c>
     </row>
     <row r="79" spans="2:17">

</xml_diff>